<commit_message>
perform new test generate fig 10 triangle force exp
</commit_message>
<xml_diff>
--- a/exp_data/triangle_force_exp_forplot.xlsx
+++ b/exp_data/triangle_force_exp_forplot.xlsx
@@ -1,40 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\dongting.ASURITE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF07A4C0-9EF0-494F-87E9-B87A331EE970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A22BABF6-7147-4788-963D-D7B3CDBD948F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -100,7 +85,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -112,7 +97,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -159,23 +144,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -211,23 +179,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -379,59 +330,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7D70AF-2BB3-41E5-A8DF-941A2EBACB16}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1.64</v>
+        <v>1.8</v>
       </c>
       <c r="B1">
-        <v>1.28</v>
+        <v>1.82</v>
       </c>
       <c r="C1">
-        <v>2</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="D1">
-        <v>1.72</v>
+        <v>1.74</v>
       </c>
       <c r="E1">
-        <v>1.42</v>
+        <v>1.9</v>
       </c>
       <c r="F1">
-        <v>1.1000000000000001</v>
+        <v>1.54</v>
       </c>
       <c r="G1">
-        <v>1.18</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1.44</v>
+        <v>1.66</v>
       </c>
       <c r="B2">
-        <v>1.3</v>
+        <v>1.9</v>
       </c>
       <c r="C2">
-        <v>1.7</v>
+        <v>1.84</v>
       </c>
       <c r="D2">
-        <v>1.38</v>
+        <v>1.96</v>
       </c>
       <c r="E2">
-        <v>1.58</v>
+        <v>1.86</v>
       </c>
       <c r="F2">
-        <v>1.1000000000000001</v>
+        <v>1.66</v>
       </c>
       <c r="G2">
-        <v>0.76</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -439,354 +390,191 @@
         <v>1.42</v>
       </c>
       <c r="B3">
-        <v>1.52</v>
+        <v>1.66</v>
       </c>
       <c r="C3">
-        <v>1.82</v>
+        <v>1.98</v>
       </c>
       <c r="D3">
-        <v>1.96</v>
+        <v>1.76</v>
       </c>
       <c r="E3">
-        <v>1.64</v>
+        <v>1.88</v>
       </c>
       <c r="F3">
-        <v>1.32</v>
+        <v>1.44</v>
       </c>
       <c r="G3">
-        <v>0.76</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1.42</v>
+        <v>1.44</v>
       </c>
       <c r="B4">
-        <v>1.42</v>
+        <v>1.98</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="D4">
-        <v>1.58</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="E4">
-        <v>1.5</v>
+        <v>1.76</v>
       </c>
       <c r="F4">
-        <v>1.3</v>
+        <v>1.86</v>
       </c>
       <c r="G4">
-        <v>0.76</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>1.68</v>
+      </c>
+      <c r="B5">
         <v>1.62</v>
       </c>
-      <c r="B5">
+      <c r="C5">
+        <v>1.84</v>
+      </c>
+      <c r="D5">
+        <v>1.9</v>
+      </c>
+      <c r="E5">
+        <v>1.62</v>
+      </c>
+      <c r="F5">
         <v>1.6</v>
       </c>
-      <c r="C5">
-        <v>1.86</v>
-      </c>
-      <c r="D5">
-        <v>1.72</v>
-      </c>
-      <c r="E5">
-        <v>1.7</v>
-      </c>
-      <c r="F5">
-        <v>1.48</v>
-      </c>
       <c r="G5">
-        <v>0.68</v>
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1.44</v>
+        <v>1.58</v>
       </c>
       <c r="B6">
-        <v>1.38</v>
+        <v>1.9</v>
       </c>
       <c r="C6">
-        <v>1.82</v>
+        <v>1.84</v>
       </c>
       <c r="D6">
-        <v>1.58</v>
+        <v>2.06</v>
       </c>
       <c r="E6">
-        <v>1.78</v>
+        <v>1.8</v>
       </c>
       <c r="F6">
-        <v>1.46</v>
+        <v>1.72</v>
       </c>
       <c r="G6">
-        <v>0.84</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1.52</v>
+        <v>1.54</v>
       </c>
       <c r="B7">
-        <v>1.5</v>
+        <v>2.04</v>
       </c>
       <c r="C7">
-        <v>1.82</v>
+        <v>1.92</v>
       </c>
       <c r="D7">
-        <v>1.9</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="E7">
-        <v>1.84</v>
+        <v>2</v>
       </c>
       <c r="F7">
         <v>1.64</v>
       </c>
       <c r="G7">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1.52</v>
+        <v>1.64</v>
       </c>
       <c r="B8">
-        <v>1.38</v>
+        <v>2.04</v>
       </c>
       <c r="C8">
-        <v>1.9</v>
+        <v>1.72</v>
       </c>
       <c r="D8">
-        <v>1.94</v>
+        <v>2.12</v>
       </c>
       <c r="E8">
-        <v>1.84</v>
+        <v>1.98</v>
       </c>
       <c r="F8">
-        <v>1.02</v>
+        <v>1.74</v>
       </c>
       <c r="G8">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1.56</v>
+        <v>1.86</v>
       </c>
       <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>1.84</v>
+      </c>
+      <c r="D9">
+        <v>2.12</v>
+      </c>
+      <c r="E9">
+        <v>1.84</v>
+      </c>
+      <c r="F9">
         <v>1.68</v>
       </c>
-      <c r="C9">
-        <v>1.54</v>
-      </c>
-      <c r="D9">
-        <v>2.02</v>
-      </c>
-      <c r="E9">
-        <v>1.66</v>
-      </c>
-      <c r="F9">
-        <v>1.2</v>
-      </c>
       <c r="G9">
-        <v>1.1000000000000001</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>1.64</v>
+      </c>
+      <c r="B10">
+        <v>2.04</v>
+      </c>
+      <c r="C10">
+        <v>2.1</v>
+      </c>
+      <c r="D10">
+        <v>2.42</v>
+      </c>
+      <c r="E10">
+        <v>1.82</v>
+      </c>
+      <c r="F10">
         <v>1.76</v>
       </c>
-      <c r="B10">
-        <v>1.78</v>
-      </c>
-      <c r="C10">
-        <v>1.64</v>
-      </c>
-      <c r="D10">
-        <v>1.72</v>
-      </c>
-      <c r="E10">
-        <v>1.64</v>
-      </c>
-      <c r="F10">
-        <v>1.26</v>
-      </c>
       <c r="G10">
-        <v>0.84</v>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1.82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063EF9A741DC20940A90CE71627684705" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="deb2d8249c24e3f660e5dc737939b14b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b81ca92bc64ec7c1c59e9a411b7bdca">
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all/>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B66C4EE5-F287-49E6-ABF7-A0F0DD317547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D155D52E-84F8-4A13-A769-5E8963700BBB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7078A4DC-B97A-4A59-A903-1CFA4F03F921}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>